<commit_message>
Can't append a commit? Lame
</commit_message>
<xml_diff>
--- a/Hardware/PinMapping.xlsx
+++ b/Hardware/PinMapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="184">
   <si>
     <t>Physical Pin #</t>
   </si>
@@ -583,6 +583,9 @@
   <si>
     <t>Do I really need these?
 (RB11 Not PPS)</t>
+  </si>
+  <si>
+    <t>Probab gonna change processor and screen on rev 2 to support MIPI</t>
   </si>
 </sst>
 </file>
@@ -1502,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1518,7 @@
     <col min="5" max="5" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2922,7 +2925,9 @@
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
-      <c r="H62" s="2"/>
+      <c r="H62" s="12" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
@@ -2936,7 +2941,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
+      <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
@@ -2950,7 +2955,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
+      <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
@@ -2979,7 +2984,8 @@
       <c r="H66" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="H62:H64"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H26:H28"/>
     <mergeCell ref="H52:H54"/>

</xml_diff>